<commit_message>
Updated documentation Added the sprint 5 backlog. Added use case scenarios for the new tasks
</commit_message>
<xml_diff>
--- a/sprints/Sprint 5/Sprint5Backlog.xlsx
+++ b/sprints/Sprint 5/Sprint5Backlog.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68E1C83-FD20-4C26-85E3-FED492491582}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +19,91 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>User Role</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>ETA</t>
+  </si>
+  <si>
+    <t>DEADLINE</t>
+  </si>
+  <si>
+    <t>Estimation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 day </t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <t>Luke</t>
+  </si>
+  <si>
+    <t>Librarian</t>
+  </si>
+  <si>
+    <t>Warehouse employee</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Luke/Carson/Tristen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">be able to check for and flag damaged rentals on all status changes, not just returns. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add ability to blacklist customers for not returning items </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add view for blacklisting customers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add DB column for flagging customer as blacklisted </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add ability to update librarians choice </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add DB table for librarians choice </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -49,8 +129,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +413,201 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" customWidth="1"/>
+    <col min="4" max="4" width="109.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F2" s="1">
+        <v>43929</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F3" s="1">
+        <v>43929</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F4" s="1">
+        <v>43929</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F5" s="1">
+        <v>43929</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F6" s="1">
+        <v>43929</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1">
+        <v>43927</v>
+      </c>
+      <c r="F7" s="1">
+        <v>43929</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>